<commit_message>
Arrowhead implemented, started on mqtt.
</commit_message>
<xml_diff>
--- a/Tests/OneToOneTest/Out/Results.xlsx
+++ b/Tests/OneToOneTest/Out/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltai Kadosa\eclipse-workspace\arrowhead-tools\Tests\OneToOneTest\Out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A4FDE-A834-4644-8784-1AC496CEA92B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D826EF-7067-4356-825C-0BC7D353063A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,6 +151,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Bandwidth</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -542,7 +567,7 @@
       <c:valAx>
         <c:axId val="486455664"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
           <c:min val="1000"/>
         </c:scaling>
@@ -695,6 +720,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Roun-Trip-Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -727,9 +777,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -746,15 +795,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$K$12:$K$16</c:f>
@@ -803,6 +866,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CBCC-4F81-B9C8-7D2B396613A7}"/>
@@ -824,15 +888,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$K$12:$K$16</c:f>
@@ -881,6 +959,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CBCC-4F81-B9C8-7D2B396613A7}"/>
@@ -902,15 +981,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$K$12:$K$16</c:f>
@@ -959,6 +1052,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-CBCC-4F81-B9C8-7D2B396613A7}"/>
@@ -973,10 +1067,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="636135040"/>
         <c:axId val="2123937568"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="636135040"/>
         <c:scaling>
@@ -1031,7 +1126,7 @@
       <c:valAx>
         <c:axId val="2123937568"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2258,16 +2353,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2294,16 +2389,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>204787</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>766762</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2669,7 +2764,7 @@
   <dimension ref="A1:N649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created additional test files.
</commit_message>
<xml_diff>
--- a/Tests/OneToOneTest/Out/Results.xlsx
+++ b/Tests/OneToOneTest/Out/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltai Kadosa\eclipse-workspace\arrowhead-tools\Tests\OneToOneTest\Out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876286B6-288B-41C1-898F-D61DF8E8DCA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314D2445-C978-48A5-BA79-EB483D65B2A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,7 +858,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Roun-Trip-Time</a:t>
+              <a:t>Round-Trip</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2581,16 +2589,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2617,15 +2625,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2992,7 +3000,7 @@
   <dimension ref="A1:O901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>